<commit_message>
My results and fixed right up hand
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Вид отклонения</t>
   </si>
@@ -70,13 +70,16 @@
     <t>0-8</t>
   </si>
   <si>
-    <t>0-9</t>
-  </si>
-  <si>
-    <t>0-6</t>
-  </si>
-  <si>
-    <t>0-5</t>
+    <t>100 - 110</t>
+  </si>
+  <si>
+    <t>80 - 90</t>
+  </si>
+  <si>
+    <t>85 - 90</t>
+  </si>
+  <si>
+    <t>170 - 180</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
         <v>14</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -476,7 +479,7 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -490,10 +493,10 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -504,10 +507,10 @@
         <v>16</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -518,10 +521,10 @@
         <v>17</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -532,10 +535,10 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -549,7 +552,7 @@
         <v>101</v>
       </c>
       <c r="D8">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -560,10 +563,10 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="D9">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -571,13 +574,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D10">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -585,13 +588,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>217</v>
+        <v>169</v>
       </c>
       <c r="D11">
-        <v>166</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>